<commit_message>
contourmap combined feature engineering
- when scaling the parameters, the stripe pattern is created
- there are a lot of differences between the contourmaps of the PCA, but some similarities can be observed
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/interpolation/combined_Fe/Area1_count.xlsx
+++ b/_CLUSTER/groups_time_area/interpolation/combined_Fe/Area1_count.xlsx
@@ -375,18 +375,18 @@
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>28228</v>
+        <v>50491</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>27185</v>
+        <v>4922</v>
       </c>
     </row>
   </sheetData>

</xml_diff>